<commit_message>
update thêm 4 từ mới ở phía dưới để tiện cho việc vẽ UC
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Hồ sơ nhân sự</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Degree</t>
-  </si>
-  <si>
-    <t>Job title, Position</t>
   </si>
   <si>
     <t>Chức vụ</t>
@@ -416,6 +413,27 @@
   </si>
   <si>
     <t>Extend information</t>
+  </si>
+  <si>
+    <t>Quá trình công tác</t>
+  </si>
+  <si>
+    <t>Working Progress</t>
+  </si>
+  <si>
+    <t>Quá trình tập sự</t>
+  </si>
+  <si>
+    <t>Probation Progress</t>
+  </si>
+  <si>
+    <t>Job title</t>
+  </si>
+  <si>
+    <t>Diễn biến lương</t>
+  </si>
+  <si>
+    <t>Wage Changes</t>
   </si>
 </sst>
 </file>
@@ -817,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,10 +850,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -843,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -859,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -867,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -894,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -902,15 +920,15 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -950,7 +968,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -963,402 +981,426 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B66" s="6" t="s">
+    </row>
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>132</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lại file English work chỗ phòng KH&QLNL
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -135,16 +135,9 @@
     <t>Supported people</t>
   </si>
   <si>
-    <t>Phòng kế hoạch</t>
-  </si>
-  <si>
     <t>Account Department</t>
   </si>
   <si>
-    <t>Planning board
-Design Department</t>
-  </si>
-  <si>
     <t>Phòng kế toán</t>
   </si>
   <si>
@@ -434,6 +427,12 @@
   </si>
   <si>
     <t>Wage Changes</t>
+  </si>
+  <si>
+    <t>Phòng kế hoạch và quản lý nhân lực</t>
+  </si>
+  <si>
+    <t>Human Resource Planning and Managing Department</t>
   </si>
 </sst>
 </file>
@@ -519,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +533,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,10 +852,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -861,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -877,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -885,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -912,7 +914,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -920,15 +922,15 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -968,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1044,363 +1046,363 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>39</v>
+      <c r="A25" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lại English Words và add phiên bản đầu tiên của use case description (7 -> 11)
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -246,9 +246,6 @@
     <t>Trang thiết bị</t>
   </si>
   <si>
-    <t>facilitate</t>
-  </si>
-  <si>
     <t>Hiện trạng</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>Human Resource Planning and Managing Department</t>
+  </si>
+  <si>
+    <t>equipment</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,10 +852,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -922,15 +922,15 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1047,10 +1047,10 @@
     </row>
     <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1202,207 +1202,207 @@
         <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update system management term
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>Hồ sơ nhân sự</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>equipment</t>
+  </si>
+  <si>
+    <t>Quản trị hệ thống</t>
+  </si>
+  <si>
+    <t>System Management</t>
   </si>
 </sst>
 </file>
@@ -837,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,6 +1409,14 @@
       </c>
       <c r="B69" s="6" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manage Document - Curriculum  fixed Manage Cirriculum Manage Project - Research  fixed Manage Project Manage probation progress fixed Manage Probation Manage Task fixed Manage Working Progress Manage Wage Change fixed Manage Wage Progress Penalty fixed discipline Equipment fixed Facilitate Add: Manage Army Rank, Manage Labor Union, Manage Union Task, Manage Communist Party Task
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8445"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="18195" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
   <si>
     <t>Hồ sơ nhân sự</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Khen thưởng/ kỉ luật</t>
   </si>
   <si>
-    <t>Reward or Penalty</t>
-  </si>
-  <si>
     <t>Quan hệ gia đình</t>
   </si>
   <si>
@@ -423,29 +420,74 @@
     <t>Diễn biến lương</t>
   </si>
   <si>
-    <t>Wage Changes</t>
-  </si>
-  <si>
     <t>Phòng kế hoạch và quản lý nhân lực</t>
   </si>
   <si>
     <t>Human Resource Planning and Managing Department</t>
   </si>
   <si>
-    <t>equipment</t>
-  </si>
-  <si>
     <t>Quản trị hệ thống</t>
   </si>
   <si>
     <t>System Management</t>
+  </si>
+  <si>
+    <t>Wage Progress</t>
+  </si>
+  <si>
+    <t>Kỉ luật</t>
+  </si>
+  <si>
+    <t>Reward</t>
+  </si>
+  <si>
+    <t>Discipline</t>
+  </si>
+  <si>
+    <t>facilitate</t>
+  </si>
+  <si>
+    <t>Quản lý công tác Đoàn</t>
+  </si>
+  <si>
+    <t>Manage Army Rank</t>
+  </si>
+  <si>
+    <t>Quản lý quân ngũ</t>
+  </si>
+  <si>
+    <t>Quản lý Công đoàn</t>
+  </si>
+  <si>
+    <t>Quản lý công tác Đảng viên</t>
+  </si>
+  <si>
+    <t>Manage Labor Union</t>
+  </si>
+  <si>
+    <t>Manage Union Task</t>
+  </si>
+  <si>
+    <t>Manage Communist Party Task</t>
+  </si>
+  <si>
+    <t>Quản lý tập sự</t>
+  </si>
+  <si>
+    <t>Manage Probation</t>
+  </si>
+  <si>
+    <t>Hướng dẫn luận văn thạc sĩ/tiến sĩ</t>
+  </si>
+  <si>
+    <t>Manage thesis guidance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,19 +496,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +518,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,22 +568,22 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,36 +885,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -880,34 +923,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -915,31 +958,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -947,7 +990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -955,7 +998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -963,7 +1006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -971,15 +1014,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -987,7 +1030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -995,7 +1038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
@@ -1003,7 +1046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1011,7 +1054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
@@ -1019,7 +1062,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
@@ -1027,401 +1070,477 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B68" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="2" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="B69" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="B76" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>140</v>
-      </c>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="10"/>
+      <c r="B81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update the last word
</commit_message>
<xml_diff>
--- a/HRM_Englishword.xlsx
+++ b/HRM_Englishword.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t>Hồ sơ nhân sự</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>Manage thesis guidance</t>
+  </si>
+  <si>
+    <t>Trung tâm phát triển phần mềm</t>
+  </si>
+  <si>
+    <t>Software Development Center</t>
   </si>
 </sst>
 </file>
@@ -887,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1527,8 +1533,12 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
-      <c r="B79" s="2"/>
+      <c r="A79" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>

</xml_diff>